<commit_message>
Full overwrite with latest ShiftBookExcel2 files
</commit_message>
<xml_diff>
--- a/bookings.xlsx
+++ b/bookings.xlsx
@@ -5,18 +5,38 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\ShiftBookExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\School\SIT_Event\SIT_ProjectHub\ShiftBookExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551BFC23-F4D0-4A0A-A776-EBC94247BF3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63D379A-C077-40CC-8442-ED751319A71F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="0" windowWidth="12070" windowHeight="9380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="70" windowWidth="11630" windowHeight="9380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>studentID</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>shift</t>
+  </si>
+  <si>
+    <t>timeStamp</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -332,14 +352,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>